<commit_message>
update code demo: https://www.codestringers.com/mastercontrol/product-style-guide/#/list-page
</commit_message>
<xml_diff>
--- a/selenium-java/expectationFile/ListPage.xlsx
+++ b/selenium-java/expectationFile/ListPage.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>text</t>
   </si>
@@ -78,9 +78,6 @@
     <t>background_color:</t>
   </si>
   <si>
-    <t>font_size: 14</t>
-  </si>
-  <si>
     <t>font_color: #18485C</t>
   </si>
   <si>
@@ -88,6 +85,12 @@
   </si>
   <si>
     <t>font_family: Open Sans</t>
+  </si>
+  <si>
+    <t>font_size: 14px</t>
+  </si>
+  <si>
+    <t>font_family: "Open Sans", sans-serif</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,16 +428,16 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -442,16 +445,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -459,16 +462,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>